<commit_message>
Small fix to excel sheet Added a regression block for ex_in vs in_in
</commit_message>
<xml_diff>
--- a/all_data.xlsx
+++ b/all_data.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zuzannaczyzowska/MED/ExploracjaTransportuKolejowego/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\koval\OneDrive\Pulpit\School\DE Project\ExploracjaTransportuKolejowego\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE2176F-7BFD-EA43-89C6-AA5D190592D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3C9450-6864-4FC5-B068-EFE2E1008B91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="-1820" windowWidth="38240" windowHeight="20780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="4" r:id="rId1"/>
+    <sheet name="Arkusz2" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1292" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="69">
   <si>
     <t>European Union - 27 countries (from 2020)</t>
   </si>
@@ -249,7 +250,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.##########"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
-    <numFmt numFmtId="170" formatCode="#,##0.0"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -363,13 +364,13 @@
     <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="170" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -706,20 +707,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3149BFEF-4CB9-2146-A1EB-EF8D3267B191}">
-  <dimension ref="A1:W388"/>
+  <dimension ref="A1:R388"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T12" sqref="T12"/>
+    <sheetView tabSelected="1" topLeftCell="A342" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="31.1640625" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
-    <col min="5" max="5" width="16.5" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D1">
         <v>0</v>
       </c>
@@ -766,7 +767,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -822,7 +823,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -841,8 +842,11 @@
       <c r="F3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="2">
-        <v>2783704</v>
+      <c r="H3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="J3" s="3">
         <v>442266046</v>
@@ -850,6 +854,12 @@
       <c r="K3" s="2">
         <v>25660</v>
       </c>
+      <c r="L3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="N3" s="2" t="s">
         <v>35</v>
       </c>
@@ -859,11 +869,14 @@
       <c r="P3" s="6">
         <v>0.4</v>
       </c>
+      <c r="Q3" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="R3" s="2">
         <v>5859</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
@@ -885,12 +898,24 @@
       <c r="G4" s="3">
         <v>3309453</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="J4" s="2">
         <v>341548691</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>35</v>
       </c>
+      <c r="L4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="N4" s="3" t="s">
         <v>35</v>
       </c>
@@ -900,9 +925,14 @@
       <c r="P4" s="5">
         <v>0.4</v>
       </c>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
@@ -924,10 +954,22 @@
       <c r="G5" s="2">
         <v>3294324</v>
       </c>
+      <c r="H5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="J5" s="3">
         <v>337331059</v>
       </c>
       <c r="K5" s="3"/>
+      <c r="L5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="N5" s="2" t="s">
         <v>35</v>
       </c>
@@ -937,9 +979,14 @@
       <c r="P5" s="6">
         <v>0.4</v>
       </c>
-      <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="Q5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
@@ -995,7 +1042,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1051,7 +1098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1107,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1163,7 +1210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1218,14 +1265,8 @@
       <c r="R10" s="3">
         <v>881</v>
       </c>
-      <c r="V10" t="s">
-        <v>54</v>
-      </c>
-      <c r="W10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1280,14 +1321,8 @@
       <c r="R11" s="2">
         <v>0</v>
       </c>
-      <c r="V11" t="s">
-        <v>55</v>
-      </c>
-      <c r="W11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1342,14 +1377,8 @@
       <c r="R12" s="3">
         <v>0</v>
       </c>
-      <c r="V12" t="s">
-        <v>56</v>
-      </c>
-      <c r="W12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1404,14 +1433,8 @@
       <c r="R13" s="2">
         <v>0</v>
       </c>
-      <c r="V13" t="s">
-        <v>57</v>
-      </c>
-      <c r="W13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1466,14 +1489,8 @@
       <c r="R14" s="3">
         <v>1908</v>
       </c>
-      <c r="V14" t="s">
-        <v>58</v>
-      </c>
-      <c r="W14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1528,14 +1545,8 @@
       <c r="R15" s="2">
         <v>2036</v>
       </c>
-      <c r="V15" t="s">
-        <v>59</v>
-      </c>
-      <c r="W15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1590,14 +1601,8 @@
       <c r="R16" s="3">
         <v>0</v>
       </c>
-      <c r="V16" t="s">
-        <v>60</v>
-      </c>
-      <c r="W16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1652,14 +1657,8 @@
       <c r="R17" s="2">
         <v>733</v>
       </c>
-      <c r="V17" t="s">
-        <v>61</v>
-      </c>
-      <c r="W17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1714,14 +1713,8 @@
       <c r="R18" s="3">
         <v>0</v>
       </c>
-      <c r="V18" t="s">
-        <v>62</v>
-      </c>
-      <c r="W18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1776,14 +1769,8 @@
       <c r="R19" s="2">
         <v>0</v>
       </c>
-      <c r="V19" t="s">
-        <v>63</v>
-      </c>
-      <c r="W19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1834,14 +1821,8 @@
       <c r="R20" s="3">
         <v>0</v>
       </c>
-      <c r="V20" t="s">
-        <v>64</v>
-      </c>
-      <c r="W20" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
@@ -1896,14 +1877,8 @@
       <c r="R21" s="2">
         <v>0</v>
       </c>
-      <c r="V21" t="s">
-        <v>65</v>
-      </c>
-      <c r="W21" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
@@ -1958,14 +1933,8 @@
       <c r="R22" s="3">
         <v>90</v>
       </c>
-      <c r="V22" t="s">
-        <v>66</v>
-      </c>
-      <c r="W22" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2020,14 +1989,8 @@
       <c r="R23" s="2">
         <v>0</v>
       </c>
-      <c r="V23" t="s">
-        <v>67</v>
-      </c>
-      <c r="W23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2082,14 +2045,8 @@
       <c r="R24" s="3">
         <v>0</v>
       </c>
-      <c r="V24" t="s">
-        <v>68</v>
-      </c>
-      <c r="W24" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2145,7 +2102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2201,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2257,7 +2214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2313,7 +2270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2369,7 +2326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2425,7 +2382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2481,7 +2438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -2535,7 +2492,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -2591,7 +2548,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -2647,7 +2604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -2703,7 +2660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -2759,7 +2716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -2815,7 +2772,7 @@
         <v>1213</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2856,7 +2813,7 @@
         <v>5865</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2895,7 +2852,7 @@
       </c>
       <c r="R39" s="2"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2932,7 +2889,7 @@
       </c>
       <c r="R40" s="2"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2988,7 +2945,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -3044,7 +3001,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -3100,7 +3057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -3156,7 +3113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -3212,7 +3169,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -3268,7 +3225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -3324,7 +3281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -3380,7 +3337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -3436,7 +3393,7 @@
         <v>1908</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -3492,7 +3449,7 @@
         <v>2043</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -3548,7 +3505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -3604,7 +3561,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -3660,7 +3617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -3716,7 +3673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -3768,7 +3725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -3824,7 +3781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -3880,7 +3837,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -3936,7 +3893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -3992,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -4048,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -4104,7 +4061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -4160,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
@@ -4216,7 +4173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -4272,7 +4229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
@@ -4328,7 +4285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>66</v>
       </c>
@@ -4384,7 +4341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>67</v>
       </c>
@@ -4438,7 +4395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>68</v>
       </c>
@@ -4494,7 +4451,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>69</v>
       </c>
@@ -4550,7 +4507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>70</v>
       </c>
@@ -4606,7 +4563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>71</v>
       </c>
@@ -4662,7 +4619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>72</v>
       </c>
@@ -4718,7 +4675,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>73</v>
       </c>
@@ -4759,7 +4716,7 @@
         <v>6697</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>74</v>
       </c>
@@ -4798,7 +4755,7 @@
       </c>
       <c r="R74" s="2"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>75</v>
       </c>
@@ -4835,7 +4792,7 @@
       </c>
       <c r="R75" s="2"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>76</v>
       </c>
@@ -4891,7 +4848,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>77</v>
       </c>
@@ -4947,7 +4904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>78</v>
       </c>
@@ -5003,7 +4960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>79</v>
       </c>
@@ -5059,7 +5016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>80</v>
       </c>
@@ -5115,7 +5072,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>81</v>
       </c>
@@ -5171,7 +5128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>82</v>
       </c>
@@ -5227,7 +5184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>83</v>
       </c>
@@ -5283,7 +5240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>84</v>
       </c>
@@ -5339,7 +5296,7 @@
         <v>2503</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>85</v>
       </c>
@@ -5395,7 +5352,7 @@
         <v>2166</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>86</v>
       </c>
@@ -5451,7 +5408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>87</v>
       </c>
@@ -5507,7 +5464,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>88</v>
       </c>
@@ -5563,7 +5520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>89</v>
       </c>
@@ -5619,7 +5576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>90</v>
       </c>
@@ -5671,7 +5628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>91</v>
       </c>
@@ -5727,7 +5684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>92</v>
       </c>
@@ -5783,7 +5740,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>93</v>
       </c>
@@ -5839,7 +5796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>94</v>
       </c>
@@ -5895,7 +5852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>95</v>
       </c>
@@ -5951,7 +5908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>96</v>
       </c>
@@ -6007,7 +5964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>97</v>
       </c>
@@ -6063,7 +6020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>98</v>
       </c>
@@ -6119,7 +6076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>99</v>
       </c>
@@ -6175,7 +6132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>100</v>
       </c>
@@ -6231,7 +6188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>102</v>
       </c>
@@ -6287,7 +6244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>103</v>
       </c>
@@ -6341,7 +6298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>104</v>
       </c>
@@ -6397,7 +6354,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>105</v>
       </c>
@@ -6453,7 +6410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>106</v>
       </c>
@@ -6509,7 +6466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>107</v>
       </c>
@@ -6565,7 +6522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>108</v>
       </c>
@@ -6621,7 +6578,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A108">
         <v>109</v>
       </c>
@@ -6662,7 +6619,7 @@
         <v>6960</v>
       </c>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A109">
         <v>110</v>
       </c>
@@ -6701,7 +6658,7 @@
       </c>
       <c r="R109" s="2"/>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>111</v>
       </c>
@@ -6738,7 +6695,7 @@
       </c>
       <c r="R110" s="2"/>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>112</v>
       </c>
@@ -6794,7 +6751,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>113</v>
       </c>
@@ -6850,7 +6807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>114</v>
       </c>
@@ -6906,7 +6863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>115</v>
       </c>
@@ -6962,7 +6919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>116</v>
       </c>
@@ -7018,7 +6975,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>117</v>
       </c>
@@ -7074,7 +7031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>118</v>
       </c>
@@ -7130,7 +7087,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>119</v>
       </c>
@@ -7186,7 +7143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>120</v>
       </c>
@@ -7242,7 +7199,7 @@
         <v>2483</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>121</v>
       </c>
@@ -7298,7 +7255,7 @@
         <v>2339</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>122</v>
       </c>
@@ -7354,7 +7311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>123</v>
       </c>
@@ -7410,7 +7367,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>124</v>
       </c>
@@ -7466,7 +7423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>125</v>
       </c>
@@ -7522,7 +7479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>126</v>
       </c>
@@ -7574,7 +7531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>127</v>
       </c>
@@ -7630,7 +7587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>128</v>
       </c>
@@ -7686,7 +7643,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>129</v>
       </c>
@@ -7742,7 +7699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>130</v>
       </c>
@@ -7798,7 +7755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>131</v>
       </c>
@@ -7854,7 +7811,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>132</v>
       </c>
@@ -7910,7 +7867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>133</v>
       </c>
@@ -7966,7 +7923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>134</v>
       </c>
@@ -8022,7 +7979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>135</v>
       </c>
@@ -8078,7 +8035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>136</v>
       </c>
@@ -8134,7 +8091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>138</v>
       </c>
@@ -8190,7 +8147,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>139</v>
       </c>
@@ -8244,7 +8201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>140</v>
       </c>
@@ -8300,7 +8257,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>141</v>
       </c>
@@ -8356,7 +8313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>142</v>
       </c>
@@ -8412,7 +8369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>143</v>
       </c>
@@ -8468,7 +8425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>144</v>
       </c>
@@ -8524,7 +8481,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>145</v>
       </c>
@@ -8565,7 +8522,7 @@
         <v>6960</v>
       </c>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>146</v>
       </c>
@@ -8604,7 +8561,7 @@
       </c>
       <c r="R144" s="2"/>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>147</v>
       </c>
@@ -8641,7 +8598,7 @@
       </c>
       <c r="R145" s="2"/>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>148</v>
       </c>
@@ -8697,7 +8654,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>149</v>
       </c>
@@ -8753,7 +8710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>150</v>
       </c>
@@ -8809,7 +8766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>151</v>
       </c>
@@ -8865,7 +8822,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>152</v>
       </c>
@@ -8921,7 +8878,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>153</v>
       </c>
@@ -8977,7 +8934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>154</v>
       </c>
@@ -9033,7 +8990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>155</v>
       </c>
@@ -9089,7 +9046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>156</v>
       </c>
@@ -9145,7 +9102,7 @@
         <v>2483</v>
       </c>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>157</v>
       </c>
@@ -9201,7 +9158,7 @@
         <v>2339</v>
       </c>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>158</v>
       </c>
@@ -9257,7 +9214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>159</v>
       </c>
@@ -9313,7 +9270,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>160</v>
       </c>
@@ -9369,7 +9326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>161</v>
       </c>
@@ -9425,7 +9382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>162</v>
       </c>
@@ -9477,7 +9434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>163</v>
       </c>
@@ -9533,7 +9490,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>164</v>
       </c>
@@ -9589,7 +9546,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>165</v>
       </c>
@@ -9645,7 +9602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A164">
         <v>166</v>
       </c>
@@ -9701,7 +9658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A165">
         <v>167</v>
       </c>
@@ -9757,7 +9714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A166">
         <v>168</v>
       </c>
@@ -9813,7 +9770,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A167">
         <v>169</v>
       </c>
@@ -9869,7 +9826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A168">
         <v>170</v>
       </c>
@@ -9925,7 +9882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A169">
         <v>171</v>
       </c>
@@ -9981,7 +9938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A170">
         <v>172</v>
       </c>
@@ -10037,7 +9994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A171">
         <v>174</v>
       </c>
@@ -10093,7 +10050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A172">
         <v>175</v>
       </c>
@@ -10147,7 +10104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A173">
         <v>176</v>
       </c>
@@ -10203,7 +10160,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A174">
         <v>177</v>
       </c>
@@ -10259,7 +10216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A175">
         <v>178</v>
       </c>
@@ -10315,7 +10272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A176">
         <v>179</v>
       </c>
@@ -10371,7 +10328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A177">
         <v>180</v>
       </c>
@@ -10427,7 +10384,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A178">
         <v>181</v>
       </c>
@@ -10468,7 +10425,7 @@
         <v>7520.1809999999996</v>
       </c>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A179">
         <v>182</v>
       </c>
@@ -10507,7 +10464,7 @@
       </c>
       <c r="R179" s="6"/>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A180">
         <v>183</v>
       </c>
@@ -10544,7 +10501,7 @@
       </c>
       <c r="R180" s="6"/>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A181">
         <v>184</v>
       </c>
@@ -10600,7 +10557,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A182">
         <v>185</v>
       </c>
@@ -10656,7 +10613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A183">
         <v>186</v>
       </c>
@@ -10712,7 +10669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A184">
         <v>187</v>
       </c>
@@ -10768,7 +10725,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A185">
         <v>188</v>
       </c>
@@ -10824,7 +10781,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A186">
         <v>189</v>
       </c>
@@ -10880,7 +10837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A187">
         <v>190</v>
       </c>
@@ -10936,7 +10893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A188">
         <v>191</v>
       </c>
@@ -10992,7 +10949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A189">
         <v>192</v>
       </c>
@@ -11048,7 +11005,7 @@
         <v>2624.181</v>
       </c>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A190">
         <v>193</v>
       </c>
@@ -11104,7 +11061,7 @@
         <v>2701</v>
       </c>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A191">
         <v>194</v>
       </c>
@@ -11160,7 +11117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A192">
         <v>195</v>
       </c>
@@ -11216,7 +11173,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A193">
         <v>196</v>
       </c>
@@ -11272,7 +11229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A194">
         <v>197</v>
       </c>
@@ -11328,7 +11285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A195">
         <v>198</v>
       </c>
@@ -11380,7 +11337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A196">
         <v>199</v>
       </c>
@@ -11436,7 +11393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A197">
         <v>200</v>
       </c>
@@ -11492,7 +11449,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A198">
         <v>201</v>
       </c>
@@ -11548,7 +11505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A199">
         <v>202</v>
       </c>
@@ -11604,7 +11561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A200">
         <v>203</v>
       </c>
@@ -11660,7 +11617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A201">
         <v>204</v>
       </c>
@@ -11716,7 +11673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A202">
         <v>205</v>
       </c>
@@ -11772,7 +11729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A203">
         <v>206</v>
       </c>
@@ -11828,7 +11785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A204">
         <v>207</v>
       </c>
@@ -11884,7 +11841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A205">
         <v>208</v>
       </c>
@@ -11940,7 +11897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A206">
         <v>210</v>
       </c>
@@ -11996,7 +11953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A207">
         <v>211</v>
       </c>
@@ -12050,7 +12007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A208">
         <v>212</v>
       </c>
@@ -12106,7 +12063,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A209">
         <v>213</v>
       </c>
@@ -12162,7 +12119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A210">
         <v>214</v>
       </c>
@@ -12218,7 +12175,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A211">
         <v>215</v>
       </c>
@@ -12274,7 +12231,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A212">
         <v>216</v>
       </c>
@@ -12330,7 +12287,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A213">
         <v>217</v>
       </c>
@@ -12371,7 +12328,7 @@
         <v>7766.1</v>
       </c>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A214">
         <v>218</v>
       </c>
@@ -12410,7 +12367,7 @@
       </c>
       <c r="R214" s="7"/>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A215">
         <v>219</v>
       </c>
@@ -12447,7 +12404,7 @@
       </c>
       <c r="R215" s="7"/>
     </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A216">
         <v>220</v>
       </c>
@@ -12503,7 +12460,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A217">
         <v>221</v>
       </c>
@@ -12559,7 +12516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A218">
         <v>222</v>
       </c>
@@ -12615,7 +12572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A219">
         <v>223</v>
       </c>
@@ -12671,7 +12628,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="220" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A220">
         <v>224</v>
       </c>
@@ -12727,7 +12684,7 @@
         <v>1104</v>
       </c>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A221">
         <v>225</v>
       </c>
@@ -12783,7 +12740,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A222">
         <v>226</v>
       </c>
@@ -12839,7 +12796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A223">
         <v>227</v>
       </c>
@@ -12895,7 +12852,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A224">
         <v>228</v>
       </c>
@@ -12951,7 +12908,7 @@
         <v>2890.1</v>
       </c>
     </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A225">
         <v>229</v>
       </c>
@@ -13007,7 +12964,7 @@
         <v>2681</v>
       </c>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A226">
         <v>230</v>
       </c>
@@ -13063,7 +13020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A227">
         <v>231</v>
       </c>
@@ -13119,7 +13076,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="228" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A228">
         <v>232</v>
       </c>
@@ -13175,7 +13132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A229">
         <v>233</v>
       </c>
@@ -13231,7 +13188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A230">
         <v>234</v>
       </c>
@@ -13283,7 +13240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A231">
         <v>235</v>
       </c>
@@ -13339,7 +13296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A232">
         <v>236</v>
       </c>
@@ -13395,7 +13352,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="233" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A233">
         <v>237</v>
       </c>
@@ -13451,7 +13408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A234">
         <v>238</v>
       </c>
@@ -13507,7 +13464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A235">
         <v>239</v>
       </c>
@@ -13563,7 +13520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A236">
         <v>240</v>
       </c>
@@ -13619,7 +13576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A237">
         <v>241</v>
       </c>
@@ -13675,7 +13632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A238">
         <v>242</v>
       </c>
@@ -13731,7 +13688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A239">
         <v>243</v>
       </c>
@@ -13787,7 +13744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A240">
         <v>244</v>
       </c>
@@ -13843,7 +13800,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A241">
         <v>246</v>
       </c>
@@ -13899,7 +13856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A242">
         <v>247</v>
       </c>
@@ -13953,7 +13910,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A243">
         <v>248</v>
       </c>
@@ -14009,7 +13966,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="244" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A244">
         <v>249</v>
       </c>
@@ -14065,7 +14022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A245">
         <v>250</v>
       </c>
@@ -14121,7 +14078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A246">
         <v>251</v>
       </c>
@@ -14177,7 +14134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A247">
         <v>252</v>
       </c>
@@ -14233,7 +14190,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="248" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A248">
         <v>253</v>
       </c>
@@ -14274,7 +14231,7 @@
         <v>7911.5649999999996</v>
       </c>
     </row>
-    <row r="249" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A249">
         <v>254</v>
       </c>
@@ -14313,7 +14270,7 @@
       </c>
       <c r="R249" s="6"/>
     </row>
-    <row r="250" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A250">
         <v>255</v>
       </c>
@@ -14350,7 +14307,7 @@
       </c>
       <c r="R250" s="6"/>
     </row>
-    <row r="251" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A251">
         <v>256</v>
       </c>
@@ -14406,7 +14363,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="252" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A252">
         <v>257</v>
       </c>
@@ -14462,7 +14419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A253">
         <v>258</v>
       </c>
@@ -14518,7 +14475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A254">
         <v>259</v>
       </c>
@@ -14574,7 +14531,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="255" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A255">
         <v>260</v>
       </c>
@@ -14630,7 +14587,7 @@
         <v>1103.5609999999999</v>
       </c>
     </row>
-    <row r="256" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A256">
         <v>261</v>
       </c>
@@ -14686,7 +14643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A257">
         <v>262</v>
       </c>
@@ -14742,7 +14699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A258">
         <v>263</v>
       </c>
@@ -14798,7 +14755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A259">
         <v>264</v>
       </c>
@@ -14854,7 +14811,7 @@
         <v>3035.0039999999999</v>
       </c>
     </row>
-    <row r="260" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A260">
         <v>265</v>
       </c>
@@ -14910,7 +14867,7 @@
         <v>2681</v>
       </c>
     </row>
-    <row r="261" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A261">
         <v>266</v>
       </c>
@@ -14966,7 +14923,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A262">
         <v>267</v>
       </c>
@@ -15022,7 +14979,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="263" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A263">
         <v>268</v>
       </c>
@@ -15078,7 +15035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A264">
         <v>269</v>
       </c>
@@ -15134,7 +15091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A265">
         <v>270</v>
       </c>
@@ -15186,7 +15143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A266">
         <v>271</v>
       </c>
@@ -15242,7 +15199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A267">
         <v>272</v>
       </c>
@@ -15298,7 +15255,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="268" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A268">
         <v>273</v>
       </c>
@@ -15354,7 +15311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A269">
         <v>274</v>
       </c>
@@ -15410,7 +15367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A270">
         <v>275</v>
       </c>
@@ -15466,7 +15423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A271">
         <v>276</v>
       </c>
@@ -15522,7 +15479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A272">
         <v>277</v>
       </c>
@@ -15578,7 +15535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="273" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A273">
         <v>278</v>
       </c>
@@ -15634,7 +15591,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A274">
         <v>279</v>
       </c>
@@ -15690,7 +15647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A275">
         <v>280</v>
       </c>
@@ -15746,7 +15703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A276">
         <v>282</v>
       </c>
@@ -15802,7 +15759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A277">
         <v>283</v>
       </c>
@@ -15856,7 +15813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="278" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A278">
         <v>284</v>
       </c>
@@ -15912,7 +15869,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="279" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A279">
         <v>285</v>
       </c>
@@ -15968,7 +15925,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="280" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A280">
         <v>286</v>
       </c>
@@ -16024,7 +15981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="281" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A281">
         <v>287</v>
       </c>
@@ -16080,7 +16037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="282" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A282">
         <v>288</v>
       </c>
@@ -16136,7 +16093,7 @@
         <v>1184</v>
       </c>
     </row>
-    <row r="283" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A283">
         <v>289</v>
       </c>
@@ -16177,7 +16134,7 @@
         <v>8018.3379999999997</v>
       </c>
     </row>
-    <row r="284" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A284">
         <v>290</v>
       </c>
@@ -16216,7 +16173,7 @@
       </c>
       <c r="R284" s="6"/>
     </row>
-    <row r="285" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A285">
         <v>291</v>
       </c>
@@ -16253,7 +16210,7 @@
       </c>
       <c r="R285" s="6"/>
     </row>
-    <row r="286" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A286">
         <v>292</v>
       </c>
@@ -16309,7 +16266,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="287" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A287">
         <v>293</v>
       </c>
@@ -16365,7 +16322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="288" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A288">
         <v>294</v>
       </c>
@@ -16421,7 +16378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="289" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A289">
         <v>295</v>
       </c>
@@ -16477,7 +16434,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="290" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A290">
         <v>296</v>
       </c>
@@ -16533,7 +16490,7 @@
         <v>1103.5609999999999</v>
       </c>
     </row>
-    <row r="291" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A291">
         <v>297</v>
       </c>
@@ -16589,7 +16546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="292" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A292">
         <v>298</v>
       </c>
@@ -16645,7 +16602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="293" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A293">
         <v>299</v>
       </c>
@@ -16701,7 +16658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="294" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A294">
         <v>300</v>
       </c>
@@ -16757,7 +16714,7 @@
         <v>3141.777</v>
       </c>
     </row>
-    <row r="295" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A295">
         <v>301</v>
       </c>
@@ -16813,7 +16770,7 @@
         <v>2681</v>
       </c>
     </row>
-    <row r="296" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A296">
         <v>302</v>
       </c>
@@ -16869,7 +16826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="297" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A297">
         <v>303</v>
       </c>
@@ -16925,7 +16882,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="298" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A298">
         <v>304</v>
       </c>
@@ -16981,7 +16938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="299" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A299">
         <v>305</v>
       </c>
@@ -17037,7 +16994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="300" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A300">
         <v>306</v>
       </c>
@@ -17089,7 +17046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="301" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A301">
         <v>307</v>
       </c>
@@ -17145,7 +17102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="302" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A302">
         <v>308</v>
       </c>
@@ -17201,7 +17158,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="303" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A303">
         <v>309</v>
       </c>
@@ -17257,7 +17214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="304" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A304">
         <v>310</v>
       </c>
@@ -17313,7 +17270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="305" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A305">
         <v>311</v>
       </c>
@@ -17369,7 +17326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="306" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A306">
         <v>312</v>
       </c>
@@ -17425,7 +17382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="307" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A307">
         <v>313</v>
       </c>
@@ -17481,7 +17438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="308" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A308">
         <v>314</v>
       </c>
@@ -17537,7 +17494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="309" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A309">
         <v>315</v>
       </c>
@@ -17593,7 +17550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="310" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A310">
         <v>316</v>
       </c>
@@ -17649,7 +17606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="311" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A311">
         <v>318</v>
       </c>
@@ -17705,7 +17662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="312" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A312">
         <v>319</v>
       </c>
@@ -17759,7 +17716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="313" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A313">
         <v>320</v>
       </c>
@@ -17815,7 +17772,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="314" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A314">
         <v>321</v>
       </c>
@@ -17871,7 +17828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="315" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A315">
         <v>322</v>
       </c>
@@ -17927,7 +17884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="316" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A316">
         <v>323</v>
       </c>
@@ -17983,7 +17940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="317" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A317">
         <v>324</v>
       </c>
@@ -18039,7 +17996,7 @@
         <v>1212</v>
       </c>
     </row>
-    <row r="318" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A318">
         <v>325</v>
       </c>
@@ -18080,7 +18037,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="319" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A319">
         <v>326</v>
       </c>
@@ -18119,7 +18076,7 @@
       </c>
       <c r="R319" s="2"/>
     </row>
-    <row r="320" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A320">
         <v>327</v>
       </c>
@@ -18156,7 +18113,7 @@
       </c>
       <c r="R320" s="2"/>
     </row>
-    <row r="321" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A321">
         <v>328</v>
       </c>
@@ -18212,7 +18169,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="322" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A322">
         <v>329</v>
       </c>
@@ -18268,7 +18225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="323" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A323">
         <v>330</v>
       </c>
@@ -18324,7 +18281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="324" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A324">
         <v>331</v>
       </c>
@@ -18380,7 +18337,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="325" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A325">
         <v>332</v>
       </c>
@@ -18436,7 +18393,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="326" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A326">
         <v>333</v>
       </c>
@@ -18492,7 +18449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="327" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A327">
         <v>334</v>
       </c>
@@ -18548,7 +18505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="328" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A328">
         <v>335</v>
       </c>
@@ -18604,7 +18561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="329" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A329">
         <v>336</v>
       </c>
@@ -18660,7 +18617,7 @@
         <v>3189.9189999999999</v>
       </c>
     </row>
-    <row r="330" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A330">
         <v>337</v>
       </c>
@@ -18716,7 +18673,7 @@
         <v>2681</v>
       </c>
     </row>
-    <row r="331" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A331">
         <v>338</v>
       </c>
@@ -18772,7 +18729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="332" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A332">
         <v>339</v>
       </c>
@@ -18828,7 +18785,7 @@
         <v>1097</v>
       </c>
     </row>
-    <row r="333" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A333">
         <v>340</v>
       </c>
@@ -18884,7 +18841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="334" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A334">
         <v>341</v>
       </c>
@@ -18940,7 +18897,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="335" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A335">
         <v>342</v>
       </c>
@@ -18992,7 +18949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="336" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A336">
         <v>343</v>
       </c>
@@ -19048,7 +19005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="337" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A337">
         <v>344</v>
       </c>
@@ -19104,7 +19061,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="338" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A338">
         <v>345</v>
       </c>
@@ -19160,7 +19117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="339" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A339">
         <v>346</v>
       </c>
@@ -19216,7 +19173,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="340" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A340">
         <v>347</v>
       </c>
@@ -19272,7 +19229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="341" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A341">
         <v>348</v>
       </c>
@@ -19328,7 +19285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="342" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A342">
         <v>349</v>
       </c>
@@ -19384,7 +19341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="343" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A343">
         <v>350</v>
       </c>
@@ -19440,7 +19397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="344" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A344">
         <v>351</v>
       </c>
@@ -19496,7 +19453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="345" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A345">
         <v>352</v>
       </c>
@@ -19552,7 +19509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="346" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A346">
         <v>354</v>
       </c>
@@ -19608,7 +19565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="347" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A347">
         <v>355</v>
       </c>
@@ -19664,7 +19621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="348" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A348">
         <v>356</v>
       </c>
@@ -19720,7 +19677,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="349" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A349">
         <v>357</v>
       </c>
@@ -19776,7 +19733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="350" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A350">
         <v>358</v>
       </c>
@@ -19832,7 +19789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="351" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A351">
         <v>359</v>
       </c>
@@ -19888,7 +19845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="352" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A352">
         <v>360</v>
       </c>
@@ -19944,113 +19901,248 @@
         <v>35</v>
       </c>
     </row>
-    <row r="353" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="353" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C353" s="4"/>
     </row>
-    <row r="354" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="354" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C354" s="4"/>
     </row>
-    <row r="355" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="355" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C355" s="4"/>
     </row>
-    <row r="356" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="356" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C356" s="4"/>
     </row>
-    <row r="357" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="357" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C357" s="4"/>
     </row>
-    <row r="358" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="358" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C358" s="4"/>
     </row>
-    <row r="359" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="359" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C359" s="4"/>
     </row>
-    <row r="360" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="360" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C360" s="4"/>
     </row>
-    <row r="361" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="361" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C361" s="4"/>
     </row>
-    <row r="362" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="362" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C362" s="4"/>
     </row>
-    <row r="363" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="363" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C363" s="4"/>
     </row>
-    <row r="364" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="364" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C364" s="4"/>
     </row>
-    <row r="365" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="365" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C365" s="4"/>
     </row>
-    <row r="366" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="366" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C366" s="4"/>
     </row>
-    <row r="367" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="367" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C367" s="4"/>
     </row>
-    <row r="368" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="368" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C368" s="4"/>
     </row>
-    <row r="369" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="369" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C369" s="4"/>
     </row>
-    <row r="370" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="370" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C370" s="4"/>
     </row>
-    <row r="371" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="371" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C371" s="4"/>
     </row>
-    <row r="372" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="372" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C372" s="4"/>
     </row>
-    <row r="373" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="373" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C373" s="4"/>
     </row>
-    <row r="374" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="374" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C374" s="4"/>
     </row>
-    <row r="375" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="375" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C375" s="4"/>
     </row>
-    <row r="376" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="376" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C376" s="4"/>
     </row>
-    <row r="377" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="377" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C377" s="4"/>
     </row>
-    <row r="378" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="378" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C378" s="4"/>
     </row>
-    <row r="379" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="379" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C379" s="4"/>
     </row>
-    <row r="380" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="380" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C380" s="4"/>
     </row>
-    <row r="381" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="381" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C381" s="4"/>
     </row>
-    <row r="382" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="382" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C382" s="4"/>
     </row>
-    <row r="383" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="383" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C383" s="4"/>
     </row>
-    <row r="384" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="384" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C384" s="4"/>
     </row>
-    <row r="385" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="385" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C385" s="4"/>
     </row>
-    <row r="386" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="386" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C386" s="4"/>
     </row>
-    <row r="387" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="387" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C387" s="4"/>
     </row>
-    <row r="388" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="388" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C388" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0216C86A-63AA-4466-82E2-FB8959F543C6}">
+  <dimension ref="B2:C16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" t="s">
+        <v>52</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>